<commit_message>
Add Accessories To Excel 23 Juli 2024 11.17 AM
</commit_message>
<xml_diff>
--- a/Data Files/Erza/Add Accessories.xlsx
+++ b/Data Files/Erza/Add Accessories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erza.akbar\Documents\Data Files Katalon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erza.akbar\git\automation1\Data Files\Erza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8522732A-3291-4B0F-9C57-B093C4004BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BF03DD-489F-41ED-B63E-F3BFCBA08920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="4185" windowWidth="15375" windowHeight="7785" xr2:uid="{1BE57175-0F35-462F-8355-E7BE32DFC19F}"/>
+    <workbookView xWindow="4680" yWindow="4125" windowWidth="15375" windowHeight="7785" xr2:uid="{1BE57175-0F35-462F-8355-E7BE32DFC19F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,9 +442,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6120229-F162-4F2C-A063-A884575E0436}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>